<commit_message>
Actually broke file for xlsx exercise
</commit_message>
<xml_diff>
--- a/01_Saturday/01_Saturday_am/data/Afghanistan_broken.cc.xlsx
+++ b/01_Saturday/01_Saturday_am/data/Afghanistan_broken.cc.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naupaka/git/Software_Carpentry/2015-10-03-ua-iplant/workshop/01_Saturday/01_Saturday_am/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Afghanistan.cc.txt" sheetId="1" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -27,12 +32,6 @@
     <t>Asia</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>continent</t>
-  </si>
-  <si>
     <t>lifeExp</t>
   </si>
   <si>
@@ -55,6 +54,30 @@
   </si>
   <si>
     <t>pop</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>2year</t>
+  </si>
+  <si>
+    <t>I need more data</t>
+  </si>
+  <si>
+    <t>asia</t>
+  </si>
+  <si>
+    <t>Asiaa</t>
+  </si>
+  <si>
+    <t>Afghnistan</t>
+  </si>
+  <si>
+    <t>726.734O548</t>
+  </si>
+  <si>
+    <t>Country information for dissertation</t>
   </si>
 </sst>
 </file>
@@ -98,6 +121,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -423,289 +451,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1997</v>
+      </c>
+      <c r="C3">
+        <v>22227415</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>41.762999999999998</v>
+      </c>
+      <c r="F3">
+        <v>635.34135100000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="C4">
+        <v>25268405</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>42.128999999999998</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2007</v>
+      </c>
+      <c r="C5">
+        <v>31889923</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>43.828000000000003</v>
+      </c>
+      <c r="F5">
+        <v>974.58033839999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1952</v>
+      </c>
+      <c r="C6">
+        <v>8425333</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>28.800999999999998</v>
+      </c>
+      <c r="F6">
+        <v>779.44531449999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>1957</v>
+      </c>
+      <c r="C7">
+        <v>9240934</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>30.332000000000001</v>
+      </c>
+      <c r="F7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>1962</v>
+      </c>
+      <c r="C8">
+        <v>10267083</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>31.997</v>
+      </c>
+      <c r="F8">
+        <v>853.10071000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1967</v>
+      </c>
+      <c r="C9">
+        <v>11537966</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>34.020000000000003</v>
+      </c>
+      <c r="F9">
+        <v>836.19713820000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1972</v>
+      </c>
+      <c r="C10">
+        <v>13079460</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10">
+        <v>739.98110580000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>1977</v>
+      </c>
+      <c r="C11">
+        <v>14880372</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>38.438000000000002</v>
+      </c>
+      <c r="F11">
+        <v>786.11335999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1982</v>
+      </c>
+      <c r="C12">
+        <v>12881816</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>39.853999999999999</v>
+      </c>
+      <c r="F12">
+        <v>978.01143879999995</v>
+      </c>
+      <c r="I12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1997</v>
-      </c>
-      <c r="C2">
-        <v>22227415</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>41.762999999999998</v>
-      </c>
-      <c r="F2">
-        <v>635.34135100000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>25268405</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>42.128999999999998</v>
-      </c>
-      <c r="F3">
-        <v>726.73405479999997</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>2007</v>
-      </c>
-      <c r="C4">
-        <v>31889923</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>43.828000000000003</v>
-      </c>
-      <c r="F4">
-        <v>974.58033839999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>1952</v>
-      </c>
-      <c r="C5">
-        <v>8425333</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>28.800999999999998</v>
-      </c>
-      <c r="F5">
-        <v>779.44531449999999</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>1957</v>
-      </c>
-      <c r="C6">
-        <v>9240934</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>30.332000000000001</v>
-      </c>
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>1962</v>
-      </c>
-      <c r="C7">
-        <v>10267083</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>31.997</v>
-      </c>
-      <c r="F7">
-        <v>853.10071000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>1967</v>
-      </c>
-      <c r="C8">
-        <v>11537966</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>34.020000000000003</v>
-      </c>
-      <c r="F8">
-        <v>836.19713820000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>1972</v>
-      </c>
-      <c r="C9">
-        <v>13079460</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9">
-        <v>739.98110580000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>1977</v>
-      </c>
-      <c r="C10">
-        <v>14880372</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>38.438000000000002</v>
-      </c>
-      <c r="F10">
-        <v>786.11335999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>1982</v>
-      </c>
-      <c r="C11">
-        <v>12881816</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>39.853999999999999</v>
-      </c>
-      <c r="F11">
-        <v>978.01143879999995</v>
-      </c>
-      <c r="G11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
         <v>1987</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>13867957</v>
       </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>40.822000000000003</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>852.39594480000005</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
         <v>1992</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>16317921</v>
       </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13">
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14">
         <v>41.673999999999999</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <v>649.34139519999997</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>